<commit_message>
added KDD dataset and other related changes
</commit_message>
<xml_diff>
--- a/resultsTables.xlsx
+++ b/resultsTables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table4" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="114">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">#2</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">literal pruning</t>
   </si>
   <si>
     <t xml:space="preserve">#3</t>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t xml:space="preserve">IDS+QCBA #6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14/7/1</t>
   </si>
   <si>
     <t xml:space="preserve">13/8/1</t>
@@ -452,7 +458,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,6 +480,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -560,11 +570,11 @@
   </sheetPr>
   <dimension ref="A2:I42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.35"/>
   </cols>
@@ -612,7 +622,7 @@
       </c>
       <c r="D3" s="1" t="str">
         <f aca="false">VLOOKUP(Table4!D2,Table4!$A$25:$C$32,3, )</f>
-        <v> </v>
+        <v>literal pruning</v>
       </c>
       <c r="E3" s="1" t="str">
         <f aca="false">VLOOKUP(Table4!E2,Table4!$A$25:$C$32,3, )</f>
@@ -1271,7 +1281,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1290,7 +1300,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -1522,7 +1532,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1535,161 +1545,242 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.37"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0.63</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>87</v>
+        <v>63</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.00124</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.00198</v>
+        <v>67</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>16.6</v>
+        <v>72</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>4.2</v>
+        <v>0.00087</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>3.4</v>
+        <v>0.00124</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.00198</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.00134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>3.6</v>
+        <v>16.6</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>1.7</v>
+        <v>4.6</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>1.5</v>
+        <v>4.2</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>3.7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>60.1</v>
+        <v>3.6</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>9</v>
+        <v>2.1</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>6.7</v>
+        <v>1.7</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1.9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>21.1</v>
+        <v>60.1</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1.3</v>
+        <v>12.2</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1.5</v>
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>8.9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C10" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>0.06</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>0.07</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="F10" s="0" t="n">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>89</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="5"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1708,29 +1799,29 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,12 +1864,12 @@
         <v>37803</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1804,85 +1895,85 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C6" s="7" t="n">
         <v>0.1088</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="7" t="n">
         <v>0.2828</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="7" t="n">
         <v>0.2425</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="7" t="n">
         <v>0.8532</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="n">
+      <c r="C7" s="7" t="n">
         <v>0.3905</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>0.6511</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="7" t="n">
         <v>0.6818</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="6" t="n">
+      <c r="C8" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <v>0.0231</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="7" t="n">
         <v>0.0215</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="7" t="n">
         <v>0.578</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,7 +1984,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1908,35 +1999,35 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1961,7 +2052,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.05248</v>
@@ -1981,7 +2072,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1991,12 +2082,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,7 +2100,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>